<commit_message>
updated data sets to recent
</commit_message>
<xml_diff>
--- a/99_data-sets-raw/Eurostat/eurostat-domestic-camping-percentage.xlsx
+++ b/99_data-sets-raw/Eurostat/eurostat-domestic-camping-percentage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lisapramann/R/IDS_Hertie_2021/97_Data_Science_Project/tourism-trends-covid/99_data-sets-raw/Eurostat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE294177-2259-4243-8FB7-B588C0C51308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A97C1A6-A3A6-934C-ADC1-B1731992F3DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15720" xr2:uid="{51C9F4F4-A8FA-BA41-BA0D-0CB4FACAB7AB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="58">
   <si>
     <t>2020-01</t>
   </si>
@@ -634,7 +634,8 @@
   <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="X15" sqref="X15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -774,8 +775,8 @@
       <c r="U2" s="4">
         <v>-42.21</v>
       </c>
-      <c r="V2" s="3" t="s">
-        <v>14</v>
+      <c r="V2" s="4">
+        <v>43.65</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
@@ -1250,8 +1251,8 @@
       <c r="U9" s="4">
         <v>29.22</v>
       </c>
-      <c r="V9" s="3" t="s">
-        <v>14</v>
+      <c r="V9" s="4">
+        <v>58.4</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
@@ -1318,8 +1319,8 @@
       <c r="U10" s="5">
         <v>-56.81</v>
       </c>
-      <c r="V10" s="6" t="s">
-        <v>14</v>
+      <c r="V10" s="5">
+        <v>-62.96</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
@@ -1454,8 +1455,8 @@
       <c r="U12" s="5">
         <v>-3.36</v>
       </c>
-      <c r="V12" s="6" t="s">
-        <v>14</v>
+      <c r="V12" s="5">
+        <v>-45.99</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
@@ -1724,10 +1725,10 @@
         <v>-16.28</v>
       </c>
       <c r="U16" s="5">
-        <v>-20.37</v>
-      </c>
-      <c r="V16" s="6" t="s">
-        <v>14</v>
+        <v>-20.46</v>
+      </c>
+      <c r="V16" s="5">
+        <v>1.65</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
@@ -1856,13 +1857,13 @@
       <c r="S18" s="5">
         <v>58.19</v>
       </c>
-      <c r="T18" s="5">
+      <c r="T18" s="4">
         <v>32.659999999999997</v>
       </c>
-      <c r="U18" s="5">
+      <c r="U18" s="4">
         <v>23.25</v>
       </c>
-      <c r="V18" s="5">
+      <c r="V18" s="4">
         <v>-11.05</v>
       </c>
     </row>
@@ -1924,13 +1925,13 @@
       <c r="S19" s="4">
         <v>23.6</v>
       </c>
-      <c r="T19" s="4">
+      <c r="T19" s="5">
         <v>133.68</v>
       </c>
-      <c r="U19" s="4">
-        <v>-6.4</v>
-      </c>
-      <c r="V19" s="4">
+      <c r="U19" s="5">
+        <v>-5.37</v>
+      </c>
+      <c r="V19" s="5">
         <v>9.5299999999999994</v>
       </c>
     </row>
@@ -1992,13 +1993,13 @@
       <c r="S20" s="5">
         <v>-31.81</v>
       </c>
-      <c r="T20" s="5">
+      <c r="T20" s="4">
         <v>-3.19</v>
       </c>
-      <c r="U20" s="5">
+      <c r="U20" s="4">
         <v>8.0399999999999991</v>
       </c>
-      <c r="V20" s="5">
+      <c r="V20" s="4">
         <v>-41.06</v>
       </c>
     </row>
@@ -2060,13 +2061,13 @@
       <c r="S21" s="4">
         <v>-40.659999999999997</v>
       </c>
-      <c r="T21" s="4">
+      <c r="T21" s="5">
         <v>-33.299999999999997</v>
       </c>
-      <c r="U21" s="4">
+      <c r="U21" s="5">
         <v>14.66</v>
       </c>
-      <c r="V21" s="4">
+      <c r="V21" s="5">
         <v>752.38</v>
       </c>
     </row>
@@ -2128,13 +2129,13 @@
       <c r="S22" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="T22" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="U22" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="V22" s="6" t="s">
+      <c r="T22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="U22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="V22" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2196,14 +2197,14 @@
       <c r="S23" s="4">
         <v>12.33</v>
       </c>
-      <c r="T23" s="4">
+      <c r="T23" s="5">
         <v>44.41</v>
       </c>
-      <c r="U23" s="4">
+      <c r="U23" s="5">
         <v>42.45</v>
       </c>
-      <c r="V23" s="3" t="s">
-        <v>14</v>
+      <c r="V23" s="5">
+        <v>46.29</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.2">
@@ -2264,13 +2265,13 @@
       <c r="S24" s="5">
         <v>26.71</v>
       </c>
-      <c r="T24" s="5">
+      <c r="T24" s="4">
         <v>25.08</v>
       </c>
-      <c r="U24" s="5">
+      <c r="U24" s="4">
         <v>22.76</v>
       </c>
-      <c r="V24" s="5">
+      <c r="V24" s="4">
         <v>39.47</v>
       </c>
     </row>
@@ -2332,13 +2333,13 @@
       <c r="S25" s="4">
         <v>-1.1000000000000001</v>
       </c>
-      <c r="T25" s="4">
+      <c r="T25" s="5">
         <v>8.9700000000000006</v>
       </c>
-      <c r="U25" s="4">
+      <c r="U25" s="5">
         <v>-7.05</v>
       </c>
-      <c r="V25" s="4">
+      <c r="V25" s="5">
         <v>-0.76</v>
       </c>
     </row>
@@ -2400,13 +2401,13 @@
       <c r="S26" s="5">
         <v>-19.41</v>
       </c>
-      <c r="T26" s="5">
+      <c r="T26" s="4">
         <v>-24.6</v>
       </c>
-      <c r="U26" s="5">
+      <c r="U26" s="4">
         <v>-24.55</v>
       </c>
-      <c r="V26" s="5">
+      <c r="V26" s="4">
         <v>-8.64</v>
       </c>
     </row>
@@ -2468,14 +2469,14 @@
       <c r="S27" s="4">
         <v>-63.1</v>
       </c>
-      <c r="T27" s="4">
+      <c r="T27" s="5">
         <v>-35.229999999999997</v>
       </c>
-      <c r="U27" s="4">
+      <c r="U27" s="5">
         <v>-27.18</v>
       </c>
-      <c r="V27" s="3" t="s">
-        <v>14</v>
+      <c r="V27" s="5">
+        <v>-25.41</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.2">
@@ -2536,14 +2537,14 @@
       <c r="S28" s="5">
         <v>51.39</v>
       </c>
-      <c r="T28" s="5">
+      <c r="T28" s="4">
         <v>90.47</v>
       </c>
-      <c r="U28" s="5">
+      <c r="U28" s="4">
         <v>65.86</v>
       </c>
-      <c r="V28" s="6" t="s">
-        <v>14</v>
+      <c r="V28" s="4">
+        <v>138.21</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
@@ -2604,14 +2605,14 @@
       <c r="S29" s="4">
         <v>-43.65</v>
       </c>
-      <c r="T29" s="4">
+      <c r="T29" s="5">
         <v>50.97</v>
       </c>
-      <c r="U29" s="4">
+      <c r="U29" s="5">
         <v>22.6</v>
       </c>
-      <c r="V29" s="3" t="s">
-        <v>14</v>
+      <c r="V29" s="5">
+        <v>63.6</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.2">
@@ -2672,13 +2673,13 @@
       <c r="S30" s="5">
         <v>12.93</v>
       </c>
-      <c r="T30" s="5">
+      <c r="T30" s="4">
         <v>28.55</v>
       </c>
-      <c r="U30" s="5">
+      <c r="U30" s="4">
         <v>20.9</v>
       </c>
-      <c r="V30" s="5">
+      <c r="V30" s="4">
         <v>26.1</v>
       </c>
     </row>
@@ -2740,13 +2741,13 @@
       <c r="S31" s="4">
         <v>-5.4</v>
       </c>
-      <c r="T31" s="4">
+      <c r="T31" s="5">
         <v>1.1599999999999999</v>
       </c>
-      <c r="U31" s="4">
+      <c r="U31" s="5">
         <v>14.47</v>
       </c>
-      <c r="V31" s="4">
+      <c r="V31" s="5">
         <v>8.39</v>
       </c>
     </row>
@@ -2808,13 +2809,13 @@
       <c r="S32" s="5">
         <v>-24.21</v>
       </c>
-      <c r="T32" s="5">
+      <c r="T32" s="4">
         <v>61.62</v>
       </c>
-      <c r="U32" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="V32" s="6" t="s">
+      <c r="U32" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="V32" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2876,13 +2877,13 @@
       <c r="S33" s="4">
         <v>1166.67</v>
       </c>
-      <c r="T33" s="3">
+      <c r="T33" s="6">
         <v>-50</v>
       </c>
-      <c r="U33" s="4">
+      <c r="U33" s="5">
         <v>-72.73</v>
       </c>
-      <c r="V33" s="3" t="s">
+      <c r="V33" s="6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2944,14 +2945,14 @@
       <c r="S34" s="5">
         <v>33.65</v>
       </c>
-      <c r="T34" s="5">
+      <c r="T34" s="4">
         <v>47.08</v>
       </c>
-      <c r="U34" s="5">
+      <c r="U34" s="4">
         <v>46.43</v>
       </c>
-      <c r="V34" s="6" t="s">
-        <v>14</v>
+      <c r="V34" s="4">
+        <v>28.93</v>
       </c>
     </row>
     <row r="35" spans="1:22" x14ac:dyDescent="0.2">

</xml_diff>